<commit_message>
Added missing abx squirrels
</commit_message>
<xml_diff>
--- a/metabolomics/metabolomics_use.xlsx
+++ b/metabolomics/metabolomics_use.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{893B4714-F39E-424D-B04B-BD9917A47A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6CE6FDE-B54C-4D1E-86D7-B72C33581BBD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D817241A-82E5-411E-B269-AA3FA1677C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E71A29DD-9D25-47BD-B0B7-A5CB770DDAA9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Acetate</t>
   </si>
@@ -97,6 +97,27 @@
   </si>
   <si>
     <t>I-S50</t>
+  </si>
+  <si>
+    <t>I-S10</t>
+  </si>
+  <si>
+    <t>I-S21</t>
+  </si>
+  <si>
+    <t>I-S30</t>
+  </si>
+  <si>
+    <t>I-S37</t>
+  </si>
+  <si>
+    <t>I-S59</t>
+  </si>
+  <si>
+    <t>I-S60</t>
+  </si>
+  <si>
+    <t>I-S61</t>
   </si>
   <si>
     <t>S-S24</t>
@@ -179,8 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -500,534 +522,771 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9599765-BDA9-4E72-B3F2-BA899DB92D8B}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="5" customWidth="1"/>
-    <col min="2" max="15" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="11.44140625" style="6" customWidth="1"/>
+    <col min="2" max="22" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="R1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>24</v>
+      <c r="T1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>245.10470000000001</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>224.98609999999999</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>148.0368</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>442.94200000000001</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>195.46119999999999</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>246.07980000000001</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>1070.1874</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
+        <v>1.6803999999999999</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1.4515</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1.9741</v>
+      </c>
+      <c r="L2" s="4">
+        <v>641.18939999999998</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N2" s="4">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="P2" s="4">
         <v>10.738200000000001</v>
       </c>
-      <c r="J2" s="3">
+      <c r="Q2" s="4">
         <v>12.148999999999999</v>
       </c>
-      <c r="K2" s="3">
+      <c r="R2" s="4">
         <v>17.069500000000001</v>
       </c>
-      <c r="L2" s="3">
+      <c r="S2" s="4">
         <v>13.904400000000001</v>
       </c>
-      <c r="M2" s="3">
+      <c r="T2" s="4">
         <v>0.50680000000000003</v>
       </c>
-      <c r="N2" s="3">
+      <c r="U2" s="4">
         <v>0.50680000000000003</v>
       </c>
-      <c r="O2" s="3">
+      <c r="V2" s="4">
         <v>0.50680000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>43.557400000000001</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>63.898800000000001</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>29.303599999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>52.232599999999998</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>88.837400000000002</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>101.6386</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>54.787500000000001</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="4">
+        <v>2.6823000000000001</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="K3" s="4">
+        <v>4.1327999999999996</v>
+      </c>
+      <c r="L3" s="4">
+        <v>20.921900000000001</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="4">
         <v>1.2539</v>
       </c>
-      <c r="J3" s="3">
+      <c r="Q3" s="4">
         <v>1.2539</v>
       </c>
-      <c r="K3" s="3">
+      <c r="R3" s="4">
         <v>1.2539</v>
       </c>
-      <c r="L3" s="3">
+      <c r="S3" s="4">
         <v>3.9613999999999998</v>
       </c>
-      <c r="M3" s="3">
+      <c r="T3" s="4">
         <v>1.2539</v>
       </c>
-      <c r="N3" s="3">
+      <c r="U3" s="4">
         <v>1.3029999999999999</v>
       </c>
-      <c r="O3" s="3">
+      <c r="V3" s="4">
         <v>1.2421</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>8.6547999999999998</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>8.6861999999999995</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>6.4063999999999997</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>168.114</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>18.085799999999999</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="4">
         <v>21.139199999999999</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>3.5274000000000001</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="4">
+        <v>30.843499999999999</v>
+      </c>
+      <c r="J4" s="4">
+        <v>41.477699999999999</v>
+      </c>
+      <c r="K4" s="4">
+        <v>41.165900000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>86.8947</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="4">
         <v>0.39589999999999997</v>
       </c>
-      <c r="J4" s="3">
+      <c r="Q4" s="4">
         <v>1.3305</v>
       </c>
-      <c r="K4" s="3">
+      <c r="R4" s="4">
         <v>0.94359999999999999</v>
       </c>
-      <c r="L4" s="3">
+      <c r="S4" s="4">
         <v>0.73619999999999997</v>
       </c>
-      <c r="M4" s="3">
+      <c r="T4" s="4">
         <v>8.7090999999999994</v>
       </c>
-      <c r="N4" s="3">
+      <c r="U4" s="4">
         <v>14.9247</v>
       </c>
-      <c r="O4" s="3">
+      <c r="V4" s="4">
         <v>8.7090999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>17.999099999999999</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>24.3232</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>5.0419</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>47.21</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>19.119499999999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <v>7.4972000000000003</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>5.3833000000000002</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="4">
+        <v>8.3096999999999994</v>
+      </c>
+      <c r="J5" s="4">
+        <v>13.7438</v>
+      </c>
+      <c r="K5" s="4">
+        <v>13.3795</v>
+      </c>
+      <c r="L5" s="4">
+        <v>122.3685</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1.2032</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1.2819</v>
+      </c>
+      <c r="P5" s="4">
         <v>0.64229999999999998</v>
       </c>
-      <c r="J5" s="3">
+      <c r="Q5" s="4">
         <v>2.5868000000000002</v>
       </c>
-      <c r="K5" s="3">
+      <c r="R5" s="4">
         <v>1.8677999999999999</v>
       </c>
-      <c r="L5" s="3">
+      <c r="S5" s="4">
         <v>4.5301999999999998</v>
       </c>
-      <c r="M5" s="3">
+      <c r="T5" s="4">
         <v>3.5425</v>
       </c>
-      <c r="N5" s="3">
+      <c r="U5" s="4">
         <v>6.7610000000000001</v>
       </c>
-      <c r="O5" s="3">
+      <c r="V5" s="4">
         <v>4.0441000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>58.884</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>40.781199999999998</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>8.3042999999999996</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>70.129099999999994</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>46.451599999999999</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="4">
         <v>11.114800000000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>22.3781</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.6238999999999999</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2.6238999999999999</v>
+      </c>
+      <c r="P6" s="4">
         <v>1.6198999999999999</v>
       </c>
-      <c r="J6" s="3">
+      <c r="Q6" s="4">
         <v>2.5829</v>
       </c>
-      <c r="K6" s="3">
+      <c r="R6" s="4">
         <v>1.6198999999999999</v>
       </c>
-      <c r="L6" s="3">
+      <c r="S6" s="4">
         <v>2.8759999999999999</v>
       </c>
-      <c r="M6" s="3">
+      <c r="T6" s="4">
         <v>3.4940000000000002</v>
       </c>
-      <c r="N6" s="3">
+      <c r="U6" s="4">
         <v>7.1760999999999999</v>
       </c>
-      <c r="O6" s="3">
+      <c r="V6" s="4">
         <v>3.4940000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>1.0446</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>1.3480000000000001</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>0.95269999999999999</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>1.0105</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>4.532</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4.4367999999999999</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.4166999999999996</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.4367999999999999</v>
+      </c>
+      <c r="L7" s="4">
+        <v>34.993499999999997</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.8881</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.56859999999999999</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1.4342999999999999</v>
+      </c>
+      <c r="P7" s="4">
         <v>0.24210000000000001</v>
       </c>
-      <c r="J7" s="3">
+      <c r="Q7" s="4">
         <v>0.47449999999999998</v>
       </c>
-      <c r="K7" s="3">
+      <c r="R7" s="4">
         <v>0.39340000000000003</v>
       </c>
-      <c r="L7" s="3">
+      <c r="S7" s="4">
         <v>0.39800000000000002</v>
       </c>
-      <c r="M7" s="3">
+      <c r="T7" s="4">
         <v>1.3011999999999999</v>
       </c>
-      <c r="N7" s="3">
+      <c r="U7" s="4">
         <v>2.1524999999999999</v>
       </c>
-      <c r="O7" s="3">
+      <c r="V7" s="4">
         <v>1.3098000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>5.65</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>8.0204000000000004</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>2.2101000000000002</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>44.959499999999998</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>4.9516</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="4">
         <v>3.9958</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>1.2023999999999999</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="4">
         <v>0.82130000000000003</v>
       </c>
-      <c r="J8" s="3">
+      <c r="Q8" s="4">
         <v>0.82130000000000003</v>
       </c>
-      <c r="K8" s="3">
+      <c r="R8" s="4">
         <v>0.82130000000000003</v>
       </c>
-      <c r="L8" s="3">
+      <c r="S8" s="4">
         <v>1.0896999999999999</v>
       </c>
-      <c r="M8" s="3">
+      <c r="T8" s="4">
         <v>1.0788</v>
       </c>
-      <c r="N8" s="3">
+      <c r="U8" s="4">
         <v>4.3390000000000004</v>
       </c>
-      <c r="O8" s="3">
+      <c r="V8" s="4">
         <v>1.0788</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>0.64529999999999998</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>0.89400000000000002</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>0.31940000000000002</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>0.5212</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <v>0.89400000000000002</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="G9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.80989999999999995</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.42230000000000001</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.80989999999999995</v>
+      </c>
+      <c r="P9" s="4">
         <v>0.3422</v>
       </c>
-      <c r="J9" s="3">
+      <c r="Q9" s="4">
         <v>0.22650000000000001</v>
       </c>
-      <c r="K9" s="3">
+      <c r="R9" s="4">
         <v>0.3533</v>
       </c>
-      <c r="L9" s="3">
+      <c r="S9" s="4">
         <v>0.17080000000000001</v>
       </c>
-      <c r="M9" s="3">
+      <c r="T9" s="4">
         <v>0.71809999999999996</v>
       </c>
-      <c r="N9" s="3">
+      <c r="U9" s="4">
         <v>1.5112000000000001</v>
       </c>
-      <c r="O9" s="3">
+      <c r="V9" s="4">
         <v>0.71809999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>37.7547</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>25.450800000000001</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>20.462700000000002</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>56.718899999999998</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>28.142099999999999</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="4">
         <v>34.314799999999998</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>59.353900000000003</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="1">
+        <v>326.41019999999997</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="4">
         <v>1.6948000000000001</v>
       </c>
-      <c r="J10" s="3">
+      <c r="Q10" s="4">
         <v>1.8169999999999999</v>
       </c>
-      <c r="K10" s="3">
+      <c r="R10" s="4">
         <v>2.1997</v>
       </c>
-      <c r="L10" s="3">
+      <c r="S10" s="4">
         <v>2.1581000000000001</v>
       </c>
-      <c r="M10" s="3">
+      <c r="T10" s="4">
         <v>1.3297000000000001</v>
       </c>
-      <c r="N10" s="3">
+      <c r="U10" s="4">
         <v>1.6749000000000001</v>
       </c>
-      <c r="O10" s="3">
+      <c r="V10" s="4">
         <v>0.6865</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>1.0555000000000001</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>1.0327</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <v>1.0327</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>1.3545</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>1.1313</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="G11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="4">
         <v>0.2288</v>
       </c>
-      <c r="J11" s="3">
+      <c r="Q11" s="4">
         <v>0.2288</v>
       </c>
-      <c r="K11" s="3">
+      <c r="R11" s="4">
         <v>0.2288</v>
       </c>
-      <c r="L11" s="3">
+      <c r="S11" s="4">
         <v>0.2288</v>
       </c>
-      <c r="M11" s="3">
+      <c r="T11" s="4">
         <v>0.254</v>
       </c>
-      <c r="N11" s="3">
+      <c r="U11" s="4">
         <v>1.4591000000000001</v>
       </c>
-      <c r="O11" s="3">
+      <c r="V11" s="4">
         <v>0.49230000000000002</v>
       </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed weird typo(?) propionate value
</commit_message>
<xml_diff>
--- a/metabolomics/metabolomics_use.xlsx
+++ b/metabolomics/metabolomics_use.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D817241A-82E5-411E-B269-AA3FA1677C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{D817241A-82E5-411E-B269-AA3FA1677C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607D2204-60E8-4944-86F8-B349F2B8F98C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E71A29DD-9D25-47BD-B0B7-A5CB770DDAA9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>Acetate</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Substrate</t>
+  </si>
+  <si>
+    <t>Antibiotics</t>
+  </si>
+  <si>
+    <t>Inulin</t>
+  </si>
+  <si>
+    <t>Saline</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -525,7 +543,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,8 +1198,8 @@
       <c r="K10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="1">
-        <v>326.41019999999997</v>
+      <c r="L10" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>32</v>
@@ -1283,10 +1301,140 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="J12" s="4"/>
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="J13" s="4"/>
+      <c r="A13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Weird propionate was from an outlier, so not typo; put back in
</commit_message>
<xml_diff>
--- a/metabolomics/metabolomics_use.xlsx
+++ b/metabolomics/metabolomics_use.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{D817241A-82E5-411E-B269-AA3FA1677C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607D2204-60E8-4944-86F8-B349F2B8F98C}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{D817241A-82E5-411E-B269-AA3FA1677C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{172EE86F-5A98-4FFA-A3C9-7FEC9EFE39AF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E71A29DD-9D25-47BD-B0B7-A5CB770DDAA9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
   <si>
     <t>Acetate</t>
   </si>
@@ -218,9 +218,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -542,897 +541,897 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9599765-BDA9-4E72-B3F2-BA899DB92D8B}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="6" customWidth="1"/>
-    <col min="2" max="22" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="11.44140625" style="5" customWidth="1"/>
+    <col min="2" max="22" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>245.10470000000001</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>224.98609999999999</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>148.0368</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>442.94200000000001</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>195.46119999999999</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>246.07980000000001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>1070.1874</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>1.6803999999999999</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>1.4515</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>1.9741</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>641.18939999999998</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <v>0.19500000000000001</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>0.15049999999999999</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>10.738200000000001</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>12.148999999999999</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="3">
         <v>17.069500000000001</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="3">
         <v>13.904400000000001</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T2" s="3">
         <v>0.50680000000000003</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="3">
         <v>0.50680000000000003</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="3">
         <v>0.50680000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>43.557400000000001</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>63.898800000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>29.303599999999999</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>52.232599999999998</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>88.837400000000002</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>101.6386</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>54.787500000000001</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>2.6823000000000001</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>2.6779999999999999</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>4.1327999999999996</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>20.921900000000001</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="4">
+      <c r="M3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="3">
         <v>1.2539</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>1.2539</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="3">
         <v>1.2539</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="3">
         <v>3.9613999999999998</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="3">
         <v>1.2539</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="3">
         <v>1.3029999999999999</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="3">
         <v>1.2421</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>8.6547999999999998</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>8.6861999999999995</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>6.4063999999999997</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>168.114</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>18.085799999999999</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>21.139199999999999</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>3.5274000000000001</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>30.843499999999999</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>41.477699999999999</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>41.165900000000001</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>86.8947</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="4">
+      <c r="M4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="3">
         <v>0.39589999999999997</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>1.3305</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="3">
         <v>0.94359999999999999</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="3">
         <v>0.73619999999999997</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="3">
         <v>8.7090999999999994</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>14.9247</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="3">
         <v>8.7090999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>17.999099999999999</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>24.3232</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>5.0419</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>47.21</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>19.119499999999999</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>7.4972000000000003</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>5.3833000000000002</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>8.3096999999999994</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>13.7438</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>13.3795</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>122.3685</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>0.91100000000000003</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>1.2032</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>1.2819</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>0.64229999999999998</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>2.5868000000000002</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="3">
         <v>1.8677999999999999</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="3">
         <v>4.5301999999999998</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="3">
         <v>3.5425</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="3">
         <v>6.7610000000000001</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="3">
         <v>4.0441000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>58.884</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>40.781199999999998</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>8.3042999999999996</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>70.129099999999994</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>46.451599999999999</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>11.114800000000001</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>22.3781</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="I6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="3">
         <v>2.6238999999999999</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>0.80769999999999997</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>2.6238999999999999</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>1.6198999999999999</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>2.5829</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <v>1.6198999999999999</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="3">
         <v>2.8759999999999999</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="3">
         <v>3.4940000000000002</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="3">
         <v>7.1760999999999999</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="3">
         <v>3.4940000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1.0446</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>1.3480000000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.95269999999999999</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1.0105</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>4.532</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="G7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="3">
         <v>4.4367999999999999</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>4.4166999999999996</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>4.4367999999999999</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>34.993499999999997</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>0.8881</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>0.56859999999999999</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>1.4342999999999999</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>0.24210000000000001</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>0.47449999999999998</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="3">
         <v>0.39340000000000003</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="3">
         <v>0.39800000000000002</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="3">
         <v>1.3011999999999999</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="3">
         <v>2.1524999999999999</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="3">
         <v>1.3098000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>5.65</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>8.0204000000000004</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>2.2101000000000002</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>44.959499999999998</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>4.9516</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>3.9958</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>1.2023999999999999</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" s="4">
+      <c r="I8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="3">
         <v>0.82130000000000003</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>0.82130000000000003</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="3">
         <v>0.82130000000000003</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="3">
         <v>1.0896999999999999</v>
       </c>
-      <c r="T8" s="4">
+      <c r="T8" s="3">
         <v>1.0788</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="3">
         <v>4.3390000000000004</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="3">
         <v>1.0788</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.64529999999999998</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.89400000000000002</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.31940000000000002</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.5212</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>0.89400000000000002</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="4">
+      <c r="G9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="3">
         <v>0.80989999999999995</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <v>0.42230000000000001</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <v>0.80989999999999995</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>0.3422</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>0.22650000000000001</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="3">
         <v>0.3533</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="3">
         <v>0.17080000000000001</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T9" s="3">
         <v>0.71809999999999996</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="3">
         <v>1.5112000000000001</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="3">
         <v>0.71809999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>37.7547</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>25.450800000000001</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>20.462700000000002</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>56.718899999999998</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>28.142099999999999</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>34.314799999999998</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>59.353900000000003</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" s="4">
+      <c r="I10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="4">
+        <v>326.41019999999997</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="3">
         <v>1.6948000000000001</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>1.8169999999999999</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="3">
         <v>2.1997</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="3">
         <v>2.1581000000000001</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10" s="3">
         <v>1.3297000000000001</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="3">
         <v>1.6749000000000001</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="3">
         <v>0.6865</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>1.0555000000000001</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>1.0327</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>1.0327</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>1.3545</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>1.1313</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P11" s="4">
+      <c r="G11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="3">
         <v>0.2288</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>0.2288</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="3">
         <v>0.2288</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="3">
         <v>0.2288</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11" s="3">
         <v>0.254</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="3">
         <v>1.4591000000000001</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11" s="3">
         <v>0.49230000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="P12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="Q12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="R12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="S12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="T12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="U12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="V12" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="P13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="R13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="S13" s="5" t="s">
+      <c r="S13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="T13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="U13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="V13" s="5" t="s">
+      <c r="V13" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>